<commit_message>
update bugs fixed status
</commit_message>
<xml_diff>
--- a/Bug/T6_Mobile.xlsx
+++ b/Bug/T6_Mobile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\OneDrive\Desktop\Talent\Docs\Bug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\Docs\Bug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2421A01-44B9-43B6-8C4B-60AEEF197AED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F90D2A7-4515-455F-B6E3-5C10DC63CBBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A52E3FAD-4BAF-45D0-98E7-77054665A105}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A52E3FAD-4BAF-45D0-98E7-77054665A105}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="60">
   <si>
     <t>STT</t>
   </si>
@@ -211,6 +211,12 @@
   </si>
   <si>
     <t>Nút menu và cái chuông dính vào nhau. Vị trí: Trong tài khoản của tôi, chi tiết xem Bug16</t>
+  </si>
+  <si>
+    <t>Tongnd</t>
+  </si>
+  <si>
+    <t>Fixed</t>
   </si>
 </sst>
 </file>
@@ -1512,21 +1518,21 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G13" sqref="G13:H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="23.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="23.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.08984375" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" customWidth="1"/>
+    <col min="1" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.7265625" customWidth="1"/>
-    <col min="6" max="6" width="13.453125" customWidth="1"/>
+    <col min="5" max="5" width="50.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="15.90625" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1555,7 +1561,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1577,7 +1583,7 @@
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:10" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1599,7 +1605,7 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:10" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1621,7 +1627,7 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:10" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1643,7 +1649,7 @@
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1665,7 +1671,7 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:10" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1687,7 +1693,7 @@
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:10" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1706,10 +1712,14 @@
       <c r="F8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:10" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G8" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1728,10 +1738,14 @@
       <c r="F9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="1:10" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G9" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1750,10 +1764,14 @@
       <c r="F10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="1:10" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G10" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1772,10 +1790,14 @@
       <c r="F11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-    </row>
-    <row r="12" spans="1:10" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G11" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1797,7 +1819,7 @@
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:10" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1816,10 +1838,14 @@
       <c r="F13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="1:10" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G13" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -1838,10 +1864,14 @@
       <c r="F14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-    </row>
-    <row r="15" spans="1:10" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G14" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -1860,10 +1890,14 @@
       <c r="F15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-    </row>
-    <row r="16" spans="1:10" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G15" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -1885,7 +1919,7 @@
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:8" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -1907,7 +1941,7 @@
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:8" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -1952,24 +1986,24 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
         <v>43</v>
       </c>
@@ -1988,19 +2022,19 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G5" t="s">
         <v>48</v>
       </c>
@@ -2019,9 +2053,9 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="5" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
         <v>52</v>
       </c>
@@ -2040,7 +2074,7 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2055,7 +2089,7 @@
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2070,24 +2104,24 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H6" t="s">
         <v>17</v>
       </c>
@@ -2106,24 +2140,24 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H7" t="s">
         <v>22</v>
       </c>
@@ -2142,19 +2176,19 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="6" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H8" t="s">
         <v>25</v>
       </c>
@@ -2173,14 +2207,14 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
         <v>27</v>
       </c>
@@ -2199,14 +2233,14 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="8" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
         <v>32</v>
       </c>
@@ -2225,19 +2259,19 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="8" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
         <v>36</v>
       </c>
@@ -2256,19 +2290,19 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
         <v>38</v>
       </c>

</xml_diff>